<commit_message>
Cleaning stuff up for manuscript
</commit_message>
<xml_diff>
--- a/biofouling/AnovaResults.xlsx
+++ b/biofouling/AnovaResults.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/Smelt-cages/biofouling/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="8_{E1E2F148-D060-4893-BC1D-36A997894EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{116BBFCB-0A65-4CD4-92F3-6549EC793EA3}"/>
+  <xr:revisionPtr revIDLastSave="188" documentId="8_{E1E2F148-D060-4893-BC1D-36A997894EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5FA0E62-D428-4EE7-A9EB-455DE6435A89}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="30450" yWindow="900" windowWidth="9600" windowHeight="5505" xr2:uid="{F7AC787C-0263-4F9C-87EE-6077924763D7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F7AC787C-0263-4F9C-87EE-6077924763D7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Anova table" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="45">
   <si>
     <t xml:space="preserve">Response </t>
   </si>
@@ -59,9 +60,6 @@
     <t>Algal biomass</t>
   </si>
   <si>
-    <t>Biofoling abundance</t>
-  </si>
-  <si>
     <t>Zooplankton Biomass</t>
   </si>
   <si>
@@ -71,15 +69,9 @@
     <t>Pseudodiaptomus CPUE</t>
   </si>
   <si>
-    <t>Diet Biomass</t>
-  </si>
-  <si>
     <t>Clod Cards</t>
   </si>
   <si>
-    <t>Biofouling Biomass</t>
-  </si>
-  <si>
     <t>Zooplankton CPUE</t>
   </si>
   <si>
@@ -108,14 +100,87 @@
   </si>
   <si>
     <t>&lt;0.0001</t>
+  </si>
+  <si>
+    <t>Biofouling Abundance</t>
+  </si>
+  <si>
+    <t>Biofoling Biomass</t>
+  </si>
+  <si>
+    <t>Diet Fullness (%BW)</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Df</t>
+  </si>
+  <si>
+    <t>SumOfSqs</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Pr(&gt;F)</t>
+  </si>
+  <si>
+    <t>Residual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Diet versus Zoop versus Biofouling - Count</t>
+  </si>
+  <si>
+    <t>Diet versus Zoop versus Biofouling - Biomass</t>
+  </si>
+  <si>
+    <t>FMWT/Cages</t>
+  </si>
+  <si>
+    <t>Scrub/Exchange</t>
+  </si>
+  <si>
+    <t>Diet/Zoop/Biofouling</t>
+  </si>
+  <si>
+    <t>Significance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zooplankton Biomass- interior scrubbed versus exchanged </t>
+  </si>
+  <si>
+    <t>Zooplankton Biomass -interior versus exterior</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zooplankton Biomass - comparison to FMWT </t>
+  </si>
+  <si>
+    <t>Diet Biomass - Scrubbed versus exchanged</t>
+  </si>
+  <si>
+    <t>Biofouling Macroinvertebrate Biomass - scrubbed versus exchanged</t>
+  </si>
+  <si>
+    <t>Inside/Outside</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -181,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -194,20 +259,33 @@
     <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D05911C-0AE8-4319-99B9-236646496676}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,15 +653,15 @@
         <v>5</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>15</v>
       </c>
       <c r="C2" s="11">
         <v>12.7658</v>
@@ -598,14 +676,14 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="8"/>
       <c r="B3" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C3" s="11">
         <v>2.7544</v>
@@ -620,7 +698,7 @@
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J3" s="1"/>
       <c r="N3" s="1"/>
@@ -628,7 +706,7 @@
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="8"/>
       <c r="B4" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" s="11">
         <v>5.3639999999999999</v>
@@ -649,7 +727,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="11">
         <v>10.164999999999999</v>
@@ -664,7 +742,7 @@
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J5" s="1"/>
       <c r="N5" s="1"/>
@@ -674,7 +752,7 @@
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="11">
         <v>2.66</v>
@@ -697,7 +775,7 @@
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="11">
         <v>11.8881</v>
@@ -713,44 +791,44 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="9">
-        <v>8.9766999999999992</v>
+        <v>12</v>
+      </c>
+      <c r="C8" s="14">
+        <v>36.552</v>
       </c>
       <c r="D8" s="8">
         <v>1</v>
       </c>
-      <c r="E8" s="9">
-        <v>34.064500000000002</v>
-      </c>
-      <c r="F8" s="10">
-        <v>2.088E-3</v>
+      <c r="E8" s="14">
+        <v>6.3491999999999997</v>
+      </c>
+      <c r="F8" s="1">
+        <v>5.3190000000000001E-2</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="9">
-        <v>0.61219999999999997</v>
+        <v>13</v>
+      </c>
+      <c r="C9" s="14">
+        <v>10.581</v>
       </c>
       <c r="D9" s="8">
         <v>1</v>
       </c>
-      <c r="E9" s="9">
-        <v>2.3233000000000001</v>
-      </c>
-      <c r="F9" s="10">
-        <v>0.18795899999999999</v>
+      <c r="E9" s="14">
+        <v>1.8379000000000001</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.23321</v>
       </c>
       <c r="G9" s="8"/>
       <c r="J9" s="2"/>
@@ -758,10 +836,10 @@
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="9">
-        <v>1.3176000000000001</v>
+        <v>14</v>
+      </c>
+      <c r="C10" s="14">
+        <v>28.785</v>
       </c>
       <c r="D10" s="8">
         <v>5</v>
@@ -772,10 +850,10 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C11" s="9">
         <v>17.973700000000001</v>
@@ -790,13 +868,13 @@
         <v>1.14E-2</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C12" s="9">
         <v>5.3962000000000003</v>
@@ -811,13 +889,13 @@
         <v>8.5629999999999998E-2</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C13" s="9">
         <v>5.9074</v>
@@ -831,55 +909,55 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="9">
-        <v>98.251999999999995</v>
+        <v>12</v>
+      </c>
+      <c r="C14" s="14">
+        <v>94.846000000000004</v>
       </c>
       <c r="D14" s="8">
         <v>3</v>
       </c>
-      <c r="E14" s="9">
-        <v>54.088999999999999</v>
+      <c r="E14" s="14">
+        <v>51.045000000000002</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="8"/>
       <c r="B15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="11">
-        <v>24.866</v>
+        <v>13</v>
+      </c>
+      <c r="C15" s="14">
+        <v>27.324999999999999</v>
       </c>
       <c r="D15" s="8">
         <v>1</v>
       </c>
-      <c r="E15" s="11">
-        <v>41.067</v>
+      <c r="E15" s="14">
+        <v>44.116999999999997</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
       <c r="B16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="9">
-        <v>33.908000000000001</v>
+        <v>14</v>
+      </c>
+      <c r="C16" s="14">
+        <v>34.685000000000002</v>
       </c>
       <c r="D16" s="8">
         <v>56</v>
@@ -890,55 +968,55 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="9">
-        <v>25.715</v>
+        <v>12</v>
+      </c>
+      <c r="C17" s="14">
+        <v>57.325000000000003</v>
       </c>
       <c r="D17" s="8">
         <v>3</v>
       </c>
-      <c r="E17" s="9">
-        <v>19.433</v>
+      <c r="E17" s="14">
+        <v>87.009</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="8"/>
       <c r="B18" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="11">
-        <v>12.21</v>
+        <v>13</v>
+      </c>
+      <c r="C18" s="14">
+        <v>6.6909999999999998</v>
       </c>
       <c r="D18" s="8">
         <v>1</v>
       </c>
-      <c r="E18" s="11">
-        <v>27.693000000000001</v>
+      <c r="E18" s="14">
+        <v>30.466000000000001</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="8"/>
       <c r="B19" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="9">
-        <v>24.701000000000001</v>
+        <v>14</v>
+      </c>
+      <c r="C19" s="14">
+        <v>12.298</v>
       </c>
       <c r="D19" s="8">
         <v>56</v>
@@ -949,10 +1027,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C20" s="11">
         <v>423.75</v>
@@ -964,16 +1042,16 @@
         <v>148.77000000000001</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="8"/>
       <c r="B21" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C21" s="9">
         <v>164.35</v>
@@ -985,16 +1063,16 @@
         <v>173.1</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="8"/>
       <c r="B22" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C22" s="9">
         <v>53.17</v>
@@ -1004,16 +1082,14 @@
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="8" t="s">
-        <v>20</v>
-      </c>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C23" s="11">
         <v>16.327000000000002</v>
@@ -1028,13 +1104,13 @@
         <v>7.7739999999999997E-3</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="8"/>
       <c r="B24" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C24" s="9">
         <v>1.8560000000000001</v>
@@ -1053,7 +1129,7 @@
     <row r="25" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="8"/>
       <c r="B25" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C25" s="9">
         <v>56.021999999999998</v>
@@ -1067,51 +1143,51 @@
     </row>
     <row r="26" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="9">
-        <v>2.399</v>
+        <v>12</v>
+      </c>
+      <c r="C26" s="15">
+        <v>9.5399999999999999E-3</v>
       </c>
       <c r="D26" s="8">
         <v>1</v>
       </c>
-      <c r="E26" s="13">
-        <v>1.7144999999999999</v>
-      </c>
-      <c r="F26" s="10">
-        <v>0.19889999999999999</v>
+      <c r="E26" s="14">
+        <v>0.72760000000000002</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.39950000000000002</v>
       </c>
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
       <c r="B27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="11">
-        <v>1.1160000000000001</v>
+        <v>13</v>
+      </c>
+      <c r="C27" s="15">
+        <v>5.3499999999999997E-3</v>
       </c>
       <c r="D27" s="8">
         <v>1</v>
       </c>
-      <c r="E27" s="11">
-        <v>0.79730000000000001</v>
-      </c>
-      <c r="F27" s="12">
-        <v>0.378</v>
+      <c r="E27" s="14">
+        <v>0.40789999999999998</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.5272</v>
       </c>
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="8"/>
       <c r="B28" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="9">
-        <v>48.978999999999999</v>
+        <v>14</v>
+      </c>
+      <c r="C28" s="15">
+        <v>0.45884999999999998</v>
       </c>
       <c r="D28" s="8">
         <v>35</v>
@@ -1126,4 +1202,676 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E599E74-222D-4BBD-9E1E-B20638DEC1A1}">
+  <dimension ref="A1:H31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="44.7265625" customWidth="1"/>
+    <col min="7" max="7" width="7.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="18">
+        <v>3.1816500622236401E-4</v>
+      </c>
+      <c r="E2" s="18">
+        <v>8.2770541966600292E-3</v>
+      </c>
+      <c r="F2" s="18">
+        <v>0.10084945062089</v>
+      </c>
+      <c r="G2" s="18">
+        <v>0.57199999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="17"/>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="18">
+        <v>2.5501831459617999E-2</v>
+      </c>
+      <c r="E3" s="18">
+        <v>0.663429468914711</v>
+      </c>
+      <c r="F3" s="18">
+        <v>8.0833707108932202</v>
+      </c>
+      <c r="G3" s="18">
+        <v>2.3E-2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="17"/>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" s="18">
+        <v>1.2619404637845701E-2</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.32829347688862898</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="17"/>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5" s="18">
+        <v>3.8439401103686099E-2</v>
+      </c>
+      <c r="E5" s="18">
+        <v>1</v>
+      </c>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="18">
+        <v>3.8546421412591202E-2</v>
+      </c>
+      <c r="E6" s="18">
+        <v>2.4020828089054602E-2</v>
+      </c>
+      <c r="F6" s="18">
+        <v>0.60201092284245505</v>
+      </c>
+      <c r="G6" s="18">
+        <v>0.65900000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="17"/>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0.989896898220746</v>
+      </c>
+      <c r="E7" s="18">
+        <v>0.61687031757199096</v>
+      </c>
+      <c r="F7" s="18">
+        <v>15.460027763357999</v>
+      </c>
+      <c r="G7" s="18">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="17"/>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0.57626494727921695</v>
+      </c>
+      <c r="E8" s="18">
+        <v>0.35910885433895501</v>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="17"/>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9" s="18">
+        <v>1.6047082669125501</v>
+      </c>
+      <c r="E9" s="18">
+        <v>1</v>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="18">
+        <v>3.5678729999999999E-2</v>
+      </c>
+      <c r="E10" s="18">
+        <v>1.5419468E-2</v>
+      </c>
+      <c r="F10" s="18">
+        <v>0.66690671899999998</v>
+      </c>
+      <c r="G10" s="18">
+        <v>0.55400000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="17"/>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="18">
+        <v>1.4757143909999999</v>
+      </c>
+      <c r="E11" s="18">
+        <v>0.63776738799999999</v>
+      </c>
+      <c r="F11" s="18">
+        <v>27.584049159999999</v>
+      </c>
+      <c r="G11" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="17"/>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12" s="18">
+        <v>0.80248246899999998</v>
+      </c>
+      <c r="E12" s="18">
+        <v>0.34681314400000002</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="17"/>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13">
+        <v>17</v>
+      </c>
+      <c r="D13" s="18">
+        <v>2.3138755899999999</v>
+      </c>
+      <c r="E13" s="18">
+        <v>1</v>
+      </c>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14" s="18">
+        <v>2.8495848219873299</v>
+      </c>
+      <c r="E14" s="18">
+        <v>0.47548352776385799</v>
+      </c>
+      <c r="F14" s="18">
+        <v>13.5433293297635</v>
+      </c>
+      <c r="G14" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="16"/>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="18">
+        <v>1.5303351520334101</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0.25535269248185299</v>
+      </c>
+      <c r="F15" s="18">
+        <v>21.819844900543501</v>
+      </c>
+      <c r="G15" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="16"/>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>23</v>
+      </c>
+      <c r="D16" s="18">
+        <v>1.6131053477787001</v>
+      </c>
+      <c r="E16" s="18">
+        <v>0.26916377975428801</v>
+      </c>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" s="16"/>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17">
+        <v>27</v>
+      </c>
+      <c r="D17" s="18">
+        <v>5.9930253217994398</v>
+      </c>
+      <c r="E17" s="18">
+        <v>1</v>
+      </c>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="18">
+        <v>0.21126956245537701</v>
+      </c>
+      <c r="E18" s="18">
+        <v>2.3544774772887699E-2</v>
+      </c>
+      <c r="F18" s="18">
+        <v>0.94677639749916398</v>
+      </c>
+      <c r="G18" s="18">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="16"/>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="18">
+        <v>1.1748570014772199</v>
+      </c>
+      <c r="E19" s="18">
+        <v>0.13093103979885301</v>
+      </c>
+      <c r="F19" s="18">
+        <v>5.2649651303661402</v>
+      </c>
+      <c r="G19" s="18">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="16"/>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>34</v>
+      </c>
+      <c r="D20" s="18">
+        <v>7.5869710551050797</v>
+      </c>
+      <c r="E20" s="18">
+        <v>0.84552418542825902</v>
+      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" s="16"/>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>36</v>
+      </c>
+      <c r="D21" s="18">
+        <v>8.9730976190376808</v>
+      </c>
+      <c r="E21" s="18">
+        <v>1</v>
+      </c>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="18">
+        <v>0.125778444290533</v>
+      </c>
+      <c r="E22" s="18">
+        <v>5.0469533373915304E-3</v>
+      </c>
+      <c r="F22" s="18">
+        <v>0.69054058435667698</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0.66200000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="16"/>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="18">
+        <v>3.0811577602940701</v>
+      </c>
+      <c r="E23" s="18">
+        <v>0.12363373970047099</v>
+      </c>
+      <c r="F23" s="18">
+        <v>16.9159707157288</v>
+      </c>
+      <c r="G23" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="H23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="16"/>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" s="18">
+        <v>10.239593078679</v>
+      </c>
+      <c r="E24" s="18">
+        <v>0.41087126457534101</v>
+      </c>
+      <c r="F24" s="18">
+        <v>28.108371939283899</v>
+      </c>
+      <c r="G24" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="H24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="16"/>
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25">
+        <v>63</v>
+      </c>
+      <c r="D25" s="18">
+        <v>11.4751285729076</v>
+      </c>
+      <c r="E25" s="18">
+        <v>0.46044804238679599</v>
+      </c>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" s="16"/>
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C26">
+        <v>67</v>
+      </c>
+      <c r="D26" s="18">
+        <v>24.921657856171201</v>
+      </c>
+      <c r="E26" s="18">
+        <v>1</v>
+      </c>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" s="18">
+        <v>8.4850004326916098E-2</v>
+      </c>
+      <c r="E27" s="18">
+        <v>4.0840915399271297E-3</v>
+      </c>
+      <c r="F27" s="18">
+        <v>0.40095642846804902</v>
+      </c>
+      <c r="G27" s="18">
+        <v>0.90300000000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" s="16"/>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" s="18">
+        <v>3.0021342571713499</v>
+      </c>
+      <c r="E28" s="18">
+        <v>0.14450195045599401</v>
+      </c>
+      <c r="F28" s="18">
+        <v>14.1865052227836</v>
+      </c>
+      <c r="G28" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="H28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" s="16"/>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="18">
+        <v>5.62646709145484</v>
+      </c>
+      <c r="E29" s="18">
+        <v>0.27081915705453602</v>
+      </c>
+      <c r="F29" s="18">
+        <v>13.293859957807401</v>
+      </c>
+      <c r="G29" s="18">
+        <v>1E-3</v>
+      </c>
+      <c r="H29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" s="16"/>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30">
+        <v>57</v>
+      </c>
+      <c r="D30" s="18">
+        <v>12.062283837456</v>
+      </c>
+      <c r="E30" s="18">
+        <v>0.58059480094954297</v>
+      </c>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="16"/>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31">
+        <v>61</v>
+      </c>
+      <c r="D31" s="18">
+        <v>20.775735190409101</v>
+      </c>
+      <c r="E31" s="18">
+        <v>1</v>
+      </c>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>